<commit_message>
added restaurant section to ResultsTemplate
</commit_message>
<xml_diff>
--- a/P2_Performer/ResultsTemplate.xlsx
+++ b/P2_Performer/ResultsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C54866-DDD7-4F2E-8905-1AB3B392C561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D968B77-CE26-4DE8-888C-2F228136383E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Hotel</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -259,109 +262,270 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -369,77 +533,23 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -449,48 +559,30 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,54 +596,69 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB9D9BD-3947-44C2-BFCC-D5F202797C3B}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,146 +996,198 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="29"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B17" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D17" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E17" s="37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
puts info for hotels into customer excel sheet
</commit_message>
<xml_diff>
--- a/P2_Performer/ResultsTemplate.xlsx
+++ b/P2_Performer/ResultsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D968B77-CE26-4DE8-888C-2F228136383E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2284E83F-EA8B-436F-B15F-9DEED6084C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -610,11 +610,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -632,33 +657,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,7 +976,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,138 +996,138 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="21"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1182,11 +1182,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1198,6 +1193,11 @@
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
weather, restaurant, and hotel info append to customer file
</commit_message>
<xml_diff>
--- a/P2_Performer/ResultsTemplate.xlsx
+++ b/P2_Performer/ResultsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2284E83F-EA8B-436F-B15F-9DEED6084C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22005290-C67E-4C2D-B7D0-0ACB1DAFB7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -186,17 +186,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -276,19 +265,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -574,6 +550,88 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -582,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,69 +654,78 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB9D9BD-3947-44C2-BFCC-D5F202797C3B}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,192 +1063,218 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="45"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="50"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="51"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="50"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="51"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1193,11 +1286,6 @@
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix customer sheet and header on template
</commit_message>
<xml_diff>
--- a/P2_Performer/ResultsTemplate.xlsx
+++ b/P2_Performer/ResultsTemplate.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C269DD-5B96-4015-99BD-FF1D0544EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,19 +71,19 @@
     <t>Airline</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Cost / ticket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -770,18 +764,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -801,9 +807,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,15 +818,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1130,18 +1124,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB9D9BD-3947-44C2-BFCC-D5F202797C3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,67 +1155,67 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="40"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="41">
+      <c r="D2" s="47">
         <f>PRODUCT(B2,C2)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="42"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="41">
+      <c r="D3" s="47">
         <f t="shared" ref="D3:D4" si="0">PRODUCT(B3,C3)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
-      <c r="D4" s="51">
+      <c r="D4" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="52"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="60" t="s">
+      <c r="E5" s="31" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="12"/>
       <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="14"/>
       <c r="E7" s="21"/>
     </row>
@@ -1229,93 +1223,93 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
@@ -1434,11 +1428,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
@@ -1453,6 +1442,11 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>